<commit_message>
Fixed drag and drop functionality and if wedding date updated then it shows on the main page.
</commit_message>
<xml_diff>
--- a/Dataset/Dataset1.xlsx
+++ b/Dataset/Dataset1.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe3062333c082e80/09 - FSD Program/14 - App Dev I/VenueFlow/VenueFLow/Dataset/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_946CF004BB691D2919DDB195D0F2E0275C78565A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9780F16B-C26F-40CD-91B8-4C24F7D606FB}"/>
+  <bookViews>
+    <workbookView xWindow="3546" yWindow="5898" windowWidth="16398" windowHeight="12396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="ok now I have to create some ex" sheetId="1" r:id="rId4"/>
+    <sheet name="ok now I have to create some ex" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -133,15 +142,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -152,36 +162,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -371,20 +388,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="21.94140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,7 +424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -415,10 +438,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -432,10 +455,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -449,10 +472,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -466,10 +489,10 @@
         <v>14</v>
       </c>
       <c r="E5" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -483,10 +506,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -500,10 +523,10 @@
         <v>19</v>
       </c>
       <c r="E7" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -517,10 +540,10 @@
         <v>8</v>
       </c>
       <c r="E8" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -534,10 +557,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -551,10 +574,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -568,10 +591,10 @@
         <v>25</v>
       </c>
       <c r="E11" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -585,10 +608,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -602,10 +625,10 @@
         <v>8</v>
       </c>
       <c r="E13" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -619,10 +642,10 @@
         <v>8</v>
       </c>
       <c r="E14" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -636,10 +659,10 @@
         <v>8</v>
       </c>
       <c r="E15" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -653,10 +676,10 @@
         <v>32</v>
       </c>
       <c r="E16" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -670,10 +693,10 @@
         <v>8</v>
       </c>
       <c r="E17" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -687,10 +710,10 @@
         <v>8</v>
       </c>
       <c r="E18" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -704,10 +727,10 @@
         <v>8</v>
       </c>
       <c r="E19" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -721,10 +744,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -738,10 +761,10 @@
         <v>8</v>
       </c>
       <c r="E21" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>